<commit_message>
finished micro bosl design
</commit_message>
<xml_diff>
--- a/nano/EDA/BoSLnano BOM Rev 0.1.0.xlsx
+++ b/nano/EDA/BoSLnano BOM Rev 0.1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\EDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\nano\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19857E7-0A72-4CFB-8430-F7E4F3447ABC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8D81A3-DEEE-42DC-9FD7-1EBEDE80EC32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -900,7 +900,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>